<commit_message>
Minor Draftbook formatting changes
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_sample_lineup_results.xlsx
+++ b/dfs-tools/build/Blog_sample_lineup_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -421,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
@@ -460,7 +460,7 @@
       </c>
       <c r="I1">
         <f>SUM(F:F)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
       </c>
       <c r="I2" s="4">
         <f>AVERAGE(B:B)</f>
-        <v>127.25384615384615</v>
+        <v>127.38571428571427</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
       </c>
       <c r="I3" s="7">
         <f>AVERAGE(C:C)</f>
-        <v>0.40826855534545664</v>
+        <v>0.4000165757670886</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
       </c>
       <c r="I4" s="10">
         <f>SUMIF(D:D,"Yes",F:F) / SUM(F:F)</f>
-        <v>0.30769230769230771</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
       </c>
       <c r="I5" s="10">
         <f>(SUM(E:E) / SUM(F:F)) - 1</f>
-        <v>-0.15384615384615385</v>
+        <v>-7.1428571428571397E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -760,6 +760,27 @@
         <v>0</v>
       </c>
       <c r="F14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43223</v>
+      </c>
+      <c r="B15" s="4">
+        <v>129.1</v>
+      </c>
+      <c r="C15" s="7">
+        <f>11219/38324</f>
+        <v>0.29274084124830396</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="8">
         <v>1</v>
       </c>
     </row>

</xml_diff>